<commit_message>
HJD and Palgrave Macmillan added.
</commit_message>
<xml_diff>
--- a/data/service-to-profession.xlsx
+++ b/data/service-to-profession.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f7c762a89876f48/R/projects/cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{FC87C90E-97C6-1340-BBC2-C0AC78C19530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AF17C2C-EF47-F344-BFFB-5BCE9E4821A3}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{FC87C90E-97C6-1340-BBC2-C0AC78C19530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C96A7DAB-563C-EC44-846B-44ABD57CB60B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -46,15 +46,9 @@
     <t>Journal of Contemporary Eastern Asia</t>
   </si>
   <si>
-    <t>2017 - Present</t>
-  </si>
-  <si>
     <t xml:space="preserve">2020 - Present </t>
   </si>
   <si>
-    <t>Korea Association for Public Diplomacy</t>
-  </si>
-  <si>
     <t>Executive Committee Member</t>
   </si>
   <si>
@@ -100,9 +94,6 @@
     <t>2019 - 2020</t>
   </si>
   <si>
-    <t>Korea Public Diplomacy Colloquium (which later became the foundation of Korea Association for Public Diplomacy)</t>
-  </si>
-  <si>
     <t>Outreach Committee Member</t>
   </si>
   <si>
@@ -113,6 +104,15 @@
   </si>
   <si>
     <t>The Hague Journal of Diplomacy</t>
+  </si>
+  <si>
+    <t>2017 - 2022</t>
+  </si>
+  <si>
+    <t>Korea Public Diplomacy Colloquium (which later became the foundation of the Korean Association for Public Diplomacy)</t>
+  </si>
+  <si>
+    <t>The Korean Association for Public Diplomacy</t>
   </si>
 </sst>
 </file>
@@ -1002,12 +1002,14 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="19.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1029,79 +1031,79 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1109,43 +1111,43 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>